<commit_message>
ver 1.2 - added feedback loop, need to fix onsset reactions to the input of the game
</commit_message>
<xml_diff>
--- a/test/test_data/dj-specs-test.xlsx
+++ b/test/test_data/dj-specs-test.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\OnSSET\test\test_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\golan\ProjectB\onsset\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D5D62A-1DA3-41F6-A75F-BB07F6D96FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="470" windowWidth="31460" windowHeight="10520" activeTab="2"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioInfo" sheetId="1" r:id="rId1"/>
@@ -161,12 +162,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -174,7 +175,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -241,7 +242,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -518,27 +519,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.3984375" customWidth="1"/>
+    <col min="7" max="7" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -567,7 +568,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -593,7 +594,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -602,26 +603,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -656,7 +657,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -694,7 +695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -732,7 +733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -759,49 +760,49 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+    <sheetView topLeftCell="S1" workbookViewId="0">
       <selection activeCell="AC12" sqref="AC12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.19921875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.19921875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.19921875" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="40.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.1796875" style="2" customWidth="1"/>
-    <col min="24" max="24" width="12.7265625" style="2" customWidth="1"/>
-    <col min="25" max="25" width="14.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="40.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.19921875" style="2" customWidth="1"/>
+    <col min="24" max="24" width="12.69921875" style="2" customWidth="1"/>
+    <col min="25" max="25" width="14.69921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.69921875" style="2" bestFit="1" customWidth="1"/>
     <col min="29" max="30" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="50" width="9.1796875" style="2" customWidth="1"/>
-    <col min="51" max="16384" width="9.1796875" style="2"/>
+    <col min="31" max="50" width="9.19921875" style="2" customWidth="1"/>
+    <col min="51" max="16384" width="9.19921875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -875,7 +876,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
fixed feedback loop + added connection to player's moves
</commit_message>
<xml_diff>
--- a/test/test_data/dj-specs-test.xlsx
+++ b/test/test_data/dj-specs-test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\golan\ProjectB\onsset\test\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D5D62A-1DA3-41F6-A75F-BB07F6D96FE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40F54E7-4C83-4BCA-93F4-73EE87E12E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioInfo" sheetId="1" r:id="rId1"/>
@@ -522,24 +522,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.3984375" customWidth="1"/>
-    <col min="7" max="7" width="10.796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.19921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.4140625" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -568,7 +568,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -606,23 +606,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.69921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.4140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.4140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.4140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -657,7 +658,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -689,13 +690,13 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -727,13 +728,13 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -747,7 +748,7 @@
         <v>0.75</v>
       </c>
       <c r="K4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L4">
         <v>2</v>
@@ -767,42 +768,42 @@
       <selection activeCell="AC12" sqref="AC12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.19921875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.19921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.4140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.4140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.4140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.4140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.19921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="40.19921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.19921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.19921875" style="2" customWidth="1"/>
-    <col min="24" max="24" width="12.69921875" style="2" customWidth="1"/>
-    <col min="25" max="25" width="14.69921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.19921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.19921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.69921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.4140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.4140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.4140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="40.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.4140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.4140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.4140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.1640625" style="2" customWidth="1"/>
+    <col min="24" max="24" width="12.6640625" style="2" customWidth="1"/>
+    <col min="25" max="25" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="29" max="30" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="50" width="9.19921875" style="2" customWidth="1"/>
-    <col min="51" max="16384" width="9.19921875" style="2"/>
+    <col min="31" max="50" width="9.1640625" style="2" customWidth="1"/>
+    <col min="51" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -876,7 +877,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>

</xml_diff>